<commit_message>
Merged PR 7561: PRI-20115 Changes to display the spot length as 30 when the plan has a spot length and is equivalized
PRI-20115 Implementation and test
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_PlansWith13And14Weeks.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_PlansWith13And14Weeks.xlsx
@@ -7564,7 +7564,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="87">
-        <v>4.5411580820137383</v>
+        <v>4.0285099091308858</v>
       </c>
       <c r="J19" s="83">
         <v>0</v>
@@ -7576,7 +7576,7 @@
         <v>2.469957622213117</v>
       </c>
       <c r="M19" s="85">
-        <v>2642.4977468916245</v>
+        <v>2978.7688923890169</v>
       </c>
       <c r="N19" s="89">
         <v>1.0291490092554654</v>
@@ -7619,7 +7619,7 @@
         <v>38</v>
       </c>
       <c r="I20" s="79">
-        <v>4.5411580820137383</v>
+        <v>4.0285099091308858</v>
       </c>
       <c r="J20" s="51" t="s">
         <v>38</v>
@@ -7631,7 +7631,7 @@
         <v>2.469957622213117</v>
       </c>
       <c r="M20" s="43">
-        <v>2642.4977468916245</v>
+        <v>2978.7688923890169</v>
       </c>
       <c r="N20" s="45" t="s">
         <v>38</v>
@@ -7966,7 +7966,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="87">
-        <v>18.164632328054957</v>
+        <v>17.6519841551721</v>
       </c>
       <c r="J29" s="83">
         <v>0</v>
@@ -7978,7 +7978,7 @@
         <v>2.469957622213117</v>
       </c>
       <c r="M29" s="85">
-        <v>2642.4977468916186</v>
+        <v>2719.2410540395717</v>
       </c>
       <c r="N29" s="89">
         <v>1.0291490092554654</v>
@@ -8021,7 +8021,7 @@
         <v>38</v>
       </c>
       <c r="I30" s="79">
-        <v>18.164632328054957</v>
+        <v>17.6519841551721</v>
       </c>
       <c r="J30" s="51" t="s">
         <v>38</v>
@@ -8033,7 +8033,7 @@
         <v>2.469957622213117</v>
       </c>
       <c r="M30" s="43">
-        <v>2642.4977468916186</v>
+        <v>2719.2410540395717</v>
       </c>
       <c r="N30" s="45" t="s">
         <v>38</v>

</xml_diff>